<commit_message>
completed actual burndown chart
</commit_message>
<xml_diff>
--- a/teamOverview/sprintBacklog/Sprint_Burndown_3.xlsx
+++ b/teamOverview/sprintBacklog/Sprint_Burndown_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riaz\OneDrive\Documents\ComSci\Year 3 Sem 1\cscc01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CCA30795-AECA-4E0C-AC26-CF1E315AF62E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{70E18640-02F9-4F8C-B2ED-B4002B63DE41}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6948" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
   <si>
     <t>Provisional</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Riaz:3</t>
+  </si>
+  <si>
+    <t>24a</t>
+  </si>
+  <si>
+    <t>24b</t>
   </si>
 </sst>
 </file>
@@ -465,16 +471,16 @@
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1648,10 +1654,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1BB781-C491-4243-859C-AAD93AE5F06E}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2142,24 +2148,24 @@
         <v>43</v>
       </c>
       <c r="D15" s="1">
-        <f>C15-SUM(K25:K35)</f>
+        <f>C15-SUM(K25:K28)</f>
         <v>43</v>
       </c>
       <c r="E15" s="1">
-        <f>D15-SUM(L25:L35)</f>
-        <v>43</v>
+        <f>D15-SUM(L25:L28)</f>
+        <v>37</v>
       </c>
       <c r="F15" s="1">
-        <f>E15-SUM(M25:M35)</f>
-        <v>43</v>
+        <f t="shared" ref="F15:H15" si="2">E15-SUM(M25:M28)</f>
+        <v>37</v>
       </c>
       <c r="G15" s="1">
-        <f>F15-SUM(N25:N35)</f>
-        <v>43</v>
+        <f t="shared" si="2"/>
+        <v>37</v>
       </c>
       <c r="H15" s="1">
-        <f>G15-SUM(O25:O35)</f>
-        <v>43</v>
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
       <c r="J15" s="1">
         <v>2</v>
@@ -2289,16 +2295,46 @@
         <v>6</v>
       </c>
     </row>
+    <row r="25" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="1">
+        <v>3</v>
+      </c>
+    </row>
     <row r="27" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J27" s="1">
+        <v>29</v>
+      </c>
+      <c r="O27" s="1">
+        <v>5</v>
+      </c>
       <c r="Q27" s="4"/>
     </row>
-    <row r="36" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J36" s="1" t="s">
+    <row r="28" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J28" s="1">
+        <v>33</v>
+      </c>
+      <c r="O28" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K36" s="1">
-        <f>SUM(K25:O35)</f>
-        <v>0</v>
+      <c r="K29" s="1">
+        <f>SUM(K25:O28)</f>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated sprint 3 burndown actual
</commit_message>
<xml_diff>
--- a/teamOverview/sprintBacklog/Sprint_Burndown_3.xlsx
+++ b/teamOverview/sprintBacklog/Sprint_Burndown_3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riaz\OneDrive\Documents\ComSci\Year 3 Sem 1\cscc01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/392e16b045ef5b88/Documents/ComSci/Year 3 Sem 1/cscc01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{70E18640-02F9-4F8C-B2ED-B4002B63DE41}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{862AA5FD-C0BD-4B0A-ACD8-19B78EF83D1B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6948" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Provisional</t>
   </si>
@@ -144,10 +144,19 @@
     <t>Riaz:3</t>
   </si>
   <si>
-    <t>24a</t>
-  </si>
-  <si>
-    <t>24b</t>
+    <t>19-David</t>
+  </si>
+  <si>
+    <t>24a-Dann</t>
+  </si>
+  <si>
+    <t>24b-Dann</t>
+  </si>
+  <si>
+    <t>22-Riaz</t>
+  </si>
+  <si>
+    <t>33-Philip</t>
   </si>
 </sst>
 </file>
@@ -474,13 +483,13 @@
                   <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1654,10 +1663,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1BB781-C491-4243-859C-AAD93AE5F06E}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2148,24 +2157,24 @@
         <v>43</v>
       </c>
       <c r="D15" s="1">
-        <f>C15-SUM(K25:K28)</f>
+        <f>C15-SUM(K25:K29)</f>
         <v>43</v>
       </c>
       <c r="E15" s="1">
-        <f>D15-SUM(L25:L28)</f>
+        <f t="shared" ref="E15:H15" si="2">D15-SUM(L25:L29)</f>
         <v>37</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" ref="F15:H15" si="2">E15-SUM(M25:M28)</f>
-        <v>37</v>
+        <f t="shared" si="2"/>
+        <v>36</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" s="1">
         <v>2</v>
@@ -2299,42 +2308,50 @@
       <c r="J25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L25" s="1">
-        <v>3</v>
+      <c r="M25" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="10:18" x14ac:dyDescent="0.3">
       <c r="J26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L26" s="1">
+      <c r="L27" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J27" s="1">
-        <v>29</v>
-      </c>
-      <c r="O27" s="1">
-        <v>5</v>
-      </c>
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J28" s="1">
-        <v>33</v>
-      </c>
-      <c r="O28" s="1">
-        <v>8</v>
+      <c r="J28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L28" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="10:18" x14ac:dyDescent="0.3">
       <c r="J29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O29" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K29" s="1">
-        <f>SUM(K25:O28)</f>
-        <v>19</v>
+      <c r="K30" s="1">
+        <f>SUM(K25:O29)</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>